<commit_message>
Atualização automática via cronjob
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/relatorio_produtos.xlsx
+++ b/dados/ADD/Dados_ADD_PF/relatorio_produtos.xlsx
@@ -53371,7 +53371,7 @@
         <v>1690</v>
       </c>
       <c r="AF326" t="s">
-        <v>1574</v>
+        <v>2710</v>
       </c>
       <c r="AG326" t="s">
         <v>3077</v>
@@ -62575,7 +62575,7 @@
         <v>1662</v>
       </c>
       <c r="AB398" t="s">
-        <v>2491</v>
+        <v>1574</v>
       </c>
       <c r="AC398" t="s">
         <v>3013</v>
@@ -62605,7 +62605,7 @@
         <v>3013</v>
       </c>
       <c r="AL398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM398">
         <v>275</v>
@@ -108631,25 +108631,25 @@
         <v>2193</v>
       </c>
       <c r="AE758" t="s">
-        <v>1781</v>
+        <v>1662</v>
       </c>
       <c r="AF758" t="s">
-        <v>2966</v>
+        <v>2478</v>
       </c>
       <c r="AG758" t="s">
-        <v>3092</v>
+        <v>2991</v>
       </c>
       <c r="AH758" t="s">
         <v>2193</v>
       </c>
       <c r="AI758" t="s">
-        <v>1662</v>
+        <v>1781</v>
       </c>
       <c r="AJ758" t="s">
-        <v>2478</v>
+        <v>2966</v>
       </c>
       <c r="AK758" t="s">
-        <v>2991</v>
+        <v>3092</v>
       </c>
       <c r="AL758">
         <v>2.95</v>

</xml_diff>